<commit_message>
instructions file and statistical guides
</commit_message>
<xml_diff>
--- a/resources/Instructions_template.xlsx
+++ b/resources/Instructions_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ab5000f3ead5dde/DocumentsHub/Projects_Programming/NuFlow/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{48B47DC1-A641-4555-8DF2-2B4CCF00AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557816C3-28C9-40D9-AAED-8808C6275C27}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{48B47DC1-A641-4555-8DF2-2B4CCF00AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C30E4E4-FDB2-46C2-A5CD-E1CB4598352D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C36C8976-3D7C-44C9-AFEB-7FD7BBE65FF5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Data</t>
   </si>
@@ -52,20 +52,148 @@
     <t>General Info</t>
   </si>
   <si>
-    <t>1. When generating the data, name the last column as</t>
-  </si>
-  <si>
-    <t>exacly like that, in all letters in lower case, the code depends on it</t>
-  </si>
-  <si>
     <t>Output Folder</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>1. Do not change the tab names</t>
+  </si>
+  <si>
+    <t>2. Do not change the columns names in any tab</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: List all subject groups/categories (e.g., `High`,</t>
+    </r>
+  </si>
+  <si>
+    <t>column named exactly `Scores`.</t>
+  </si>
+  <si>
+    <t>`Low`, `HC`). Ensure your experiment data file has a</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Output Folder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: In the cell below this column header,</t>
+    </r>
+  </si>
+  <si>
+    <t>provide the full path to the folder where result files and</t>
+  </si>
+  <si>
+    <t>plots should be saved.</t>
+  </si>
+  <si>
+    <t>`.xlsx` or `.csv`).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide the full path to the experiment file (e.g., a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: An identifier for each experiment; this can</t>
+    </r>
+  </si>
+  <si>
+    <t>be a string or a number.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +211,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -148,17 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,8 +298,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -186,10 +331,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,22 +653,22 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="14.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -541,7 +682,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,40 +710,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B82FA30-D19B-4A0E-8A62-9B1783C646ED}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="50" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>